<commit_message>
Attempting removal of all Caledar objects (required ones change to LocalDate). Unfinished as of commit/branch
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -67,7 +67,7 @@
     <t>103-EAGLES-CROWE</t>
   </si>
   <si>
-    <t>Plays in afternoon in Y league</t>
+    <t>After 12:00</t>
   </si>
   <si>
     <t>104-GAUCHOS</t>
@@ -104,7 +104,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -167,11 +167,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +225,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -295,10 +290,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -307,19 +298,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -450,7 +433,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H8" activeCellId="0" pane="topLeft" sqref="H8"/>
+      <selection activeCell="H5" activeCellId="0" pane="topLeft" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -530,7 +513,7 @@
       <c r="A4" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
@@ -544,16 +527,16 @@
       <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="19" t="n">
+      <c r="A5" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="15" t="s">
         <v>15</v>
       </c>
@@ -576,7 +559,7 @@
       <c r="A6" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -584,22 +567,22 @@
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="16" t="n">
+      <c r="F6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.45" outlineLevel="0" r="7">
       <c r="A7" s="11" t="n">
         <v>105</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
@@ -613,18 +596,18 @@
       <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.85" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="8">
       <c r="A8" s="11" t="n">
         <v>106</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
@@ -638,16 +621,16 @@
       <c r="G8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="9">
       <c r="A9" s="11" t="n">
         <v>107</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="15" t="s">
         <v>24</v>
       </c>
@@ -661,10 +644,10 @@
       <c r="G9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
@@ -672,13 +655,8 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5,H8">
-    <cfRule aboveAverage="0" bottom="0" dxfId="1" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="duplicateValues" percent="0" priority="4" rank="0" text="" type="duplicateValues">
+    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reworked parser to comply with new input, reworked DateConstraint to utalize the time slots and dates of conference, added in functionality for days of week ("only thursday, no saturday"), adjusted book2.xlsx for input.
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -61,13 +61,13 @@
     <t>C</t>
   </si>
   <si>
-    <t>Xr 4:40-5:40</t>
+    <t>no 4:40pm-5:40pm</t>
   </si>
   <si>
     <t>103-EAGLES-CROWE</t>
   </si>
   <si>
-    <t>After 12:00</t>
+    <t>Only After 12:00pm</t>
   </si>
   <si>
     <t>104-GAUCHOS</t>
@@ -76,13 +76,13 @@
     <t>I</t>
   </si>
   <si>
-    <t>Xd 1/12/13-1/20/13, xd 3/3/13</t>
+    <t>no 1/12/14-1/20/14, no 3/3/14</t>
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
   </si>
   <si>
-    <t>xd 2/17/13</t>
+    <t>no 2/17/13</t>
   </si>
   <si>
     <t>Irish 2, Bears 3</t>
@@ -94,7 +94,7 @@
     <t>107-SHOOTIN TIGERS-JENNINGS</t>
   </si>
   <si>
-    <t>TH ONLY, NO Sat</t>
+    <t>only thursday, no saturday</t>
   </si>
 </sst>
 </file>
@@ -315,22 +315,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <sz val="11"/>
@@ -433,7 +418,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H5" activeCellId="0" pane="topLeft" sqref="H5"/>
+      <selection activeCell="H6" activeCellId="0" pane="topLeft" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,7 +494,7 @@
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.85" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="4">
       <c r="A4" s="11" t="n">
         <v>102</v>
       </c>
@@ -532,7 +517,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="5">
       <c r="A5" s="11" t="n">
         <v>103</v>
       </c>
@@ -555,7 +540,7 @@
       </c>
       <c r="I5" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.45" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="6">
       <c r="A6" s="11" t="n">
         <v>104</v>
       </c>
@@ -578,7 +563,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.45" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="7">
       <c r="A7" s="11" t="n">
         <v>105</v>
       </c>
@@ -626,7 +611,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.45" outlineLevel="0" r="9">
       <c r="A9" s="11" t="n">
         <v>107</v>
       </c>
@@ -656,7 +641,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
+    <cfRule aboveAverage="0" bottom="0" dxfId="1" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Yes, teams playing themselves is already taken care of (specifically, when the Matches are all constructed). If anyone else runs into a problem where during the build process, it says we have the wrong version of something, go into File > Project Structure > Libraries and delete XMLBeans 2.2 (keep 2.3).
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -67,7 +67,7 @@
     <t>103-EAGLES-CROWE</t>
   </si>
   <si>
-    <t>Only After 12:00pm</t>
+    <t>Only After 5:00pm</t>
   </si>
   <si>
     <t>104-GAUCHOS</t>
@@ -76,13 +76,13 @@
     <t>I</t>
   </si>
   <si>
-    <t>no 1/12/14-1/20/14, no 3/3/14</t>
+    <t>no 1/12/14-1/20/14, no 1/20/14</t>
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
   </si>
   <si>
-    <t>no 2/17/13</t>
+    <t>No 1/17/14</t>
   </si>
   <si>
     <t>Irish 2, Bears 3</t>
@@ -418,7 +418,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H6" activeCellId="0" pane="topLeft" sqref="H6"/>
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -477,7 +477,9 @@
       <c r="A3" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
@@ -494,11 +496,13 @@
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="4">
       <c r="A4" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
@@ -517,11 +521,13 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="5">
       <c r="A5" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C5" s="15" t="s">
         <v>15</v>
       </c>
@@ -540,11 +546,13 @@
       </c>
       <c r="I5" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="6">
       <c r="A6" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -563,11 +571,13 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="7">
       <c r="A7" s="11" t="n">
         <v>105</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
@@ -588,11 +598,13 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="8">
       <c r="A8" s="11" t="n">
         <v>106</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
@@ -611,11 +623,13 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.45" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
       <c r="A9" s="11" t="n">
         <v>107</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C9" s="15" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Date constraints and time constraints are still buggy-- it's scheduling people for times they aren't available. Not sure what's going on yet, but I've squashed a couple bugs already...
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -67,7 +67,7 @@
     <t>103-EAGLES-CROWE</t>
   </si>
   <si>
-    <t>Only After 5:00pm</t>
+    <t>Only After 7:00pm</t>
   </si>
   <si>
     <t>104-GAUCHOS</t>
@@ -76,13 +76,13 @@
     <t>I</t>
   </si>
   <si>
-    <t>no 1/12/14-1/20/14, no 1/20/14</t>
+    <t>no 1/10/14-1/13/14, no 1/6/14</t>
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
   </si>
   <si>
-    <t>No 1/17/14</t>
+    <t>No 1/12/14</t>
   </si>
   <si>
     <t>Irish 2, Bears 3</t>
@@ -418,7 +418,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
+      <selection activeCell="H5" activeCellId="0" pane="topLeft" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Neither requesting a weekday nor "before X" appear to be functional, but I've just code reviewed and bughunted the HELL out of all of DateConstraint. It looks like "only date" is working now, as are "after X" and time-based requests. #1140933 #1171259 #1175999
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -82,7 +82,7 @@
     <t>105-IRISH-WEBSTER 1</t>
   </si>
   <si>
-    <t>No 1/12/14</t>
+    <t>No 1/12/14, only before 10:00pm</t>
   </si>
   <si>
     <t>Irish 2, Bears 3</t>
@@ -418,7 +418,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H5" activeCellId="0" pane="topLeft" sqref="H5"/>
+      <selection activeCell="H8" activeCellId="0" pane="topLeft" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="3">
       <c r="A3" s="11" t="n">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Before/after, time-based, date-based, and day-based constraints should all be working now, along with all constraint categories (prefer, no, only). Conference primary days should be implementable as preferred dates-- it'd be the same as saying for everyone in a conference, "pref [day of week]", just automatic.
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
@@ -61,7 +61,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>no 4:40pm-5:40pm</t>
+    <t>no 5:40pm-6:40pm</t>
   </si>
   <si>
     <t>103-EAGLES-CROWE</t>
@@ -91,10 +91,13 @@
     <t>106-PATRIOTS</t>
   </si>
   <si>
+    <t>no 6:40pm-7:40pm</t>
+  </si>
+  <si>
     <t>107-SHOOTIN TIGERS-JENNINGS</t>
   </si>
   <si>
-    <t>only thursday, no saturday</t>
+    <t>pref thursday, no saturday</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H8" activeCellId="0" pane="topLeft" sqref="H8"/>
+      <selection activeCell="H18" activeCellId="0" pane="topLeft" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,7 +622,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I8" s="17"/>
     </row>
@@ -631,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="12" t="s">
@@ -644,7 +647,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I9" s="17"/>
     </row>

</xml_diff>